<commit_message>
some initial chart work with highcharts
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Adjust slider that does not reposition if, after slideing, the weight of the item is unchanged</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Think about Accordion</t>
+  </si>
+  <si>
+    <t>Turn Chart.component into a directive</t>
+  </si>
+  <si>
+    <t>Inject js lib</t>
   </si>
 </sst>
 </file>
@@ -477,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C28"/>
+  <dimension ref="B1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,6 +622,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>8</v>
@@ -643,6 +657,17 @@
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some progres with charts
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Adjust slider that does not reposition if, after slideing, the weight of the item is unchanged</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Inject js lib</t>
+  </si>
+  <si>
+    <t>try to insert js lib references in the components rather than in index.html</t>
   </si>
 </sst>
 </file>
@@ -483,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C30"/>
+  <dimension ref="B1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,15 +635,12 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
@@ -664,9 +664,17 @@
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>26</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C32" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
asset pie charts working
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>Adjust slider that does not reposition if, after slideing, the weight of the item is unchanged</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>try to insert js lib references in the components rather than in index.html</t>
+  </si>
+  <si>
+    <t>Change Highstocks with Highcharts</t>
   </si>
 </sst>
 </file>
@@ -486,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C32"/>
+  <dimension ref="B1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,7 +614,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -619,36 +622,36 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>7</v>
       </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
@@ -656,7 +659,7 @@
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
@@ -664,7 +667,7 @@
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
@@ -672,9 +675,17 @@
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>26</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C34" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
charts and comparator working
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Adjust slider that does not reposition if, after slideing, the weight of the item is unchanged</t>
   </si>
@@ -106,13 +106,25 @@
   </si>
   <si>
     <t>Change Highstocks with Highcharts</t>
+  </si>
+  <si>
+    <t>Study MongoDB schema design</t>
+  </si>
+  <si>
+    <t>Unsubscribe change events on Destroy</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>When no search selection criteria is selected retrieve all sheets from Factory and not like now where no sheets are shown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +143,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,10 +174,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C34"/>
+  <dimension ref="B1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +572,7 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -596,78 +615,94 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="C15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="C17" t="s">
-        <v>12</v>
+      <c r="C18" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="C20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>25</v>
       </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>8</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
@@ -675,7 +710,7 @@
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
@@ -683,9 +718,17 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>26</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>